<commit_message>
added more functionality, bug fixes, more comments in code, altered map and items in world.xlsx
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>StartingRoom</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>FindGiantSnakeRoom1</t>
+  </si>
+  <si>
+    <t>FindSwordRoom1</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="E12:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -436,6 +439,9 @@
       </c>
     </row>
     <row r="14" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
       <c r="H14" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
refactored story line, initial commit
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfarmer/Coding/Python/adventuregame/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfarmer/Coding/com.despoina/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="59240" yWindow="7960" windowWidth="26740" windowHeight="18640" tabRatio="500"/>
+    <workbookView xWindow="16640" yWindow="460" windowWidth="15980" windowHeight="18640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map.txt" sheetId="1" r:id="rId1"/>
@@ -27,63 +27,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>StartingRoom</t>
-  </si>
-  <si>
-    <t>GiantPlantRoom1</t>
-  </si>
-  <si>
-    <t>LeaveCaveRoom</t>
-  </si>
-  <si>
-    <t>FindRustyBootsRoom1</t>
-  </si>
-  <si>
-    <t>EmptyCavePath1</t>
-  </si>
-  <si>
-    <t>HallOfFameCooridor1</t>
-  </si>
-  <si>
-    <t>EmptyCavePath2</t>
-  </si>
-  <si>
-    <t>FindRustyHelmet1</t>
-  </si>
-  <si>
-    <t>MerchantRoom1</t>
-  </si>
-  <si>
-    <t>FindKnifeRoom1</t>
-  </si>
-  <si>
-    <t>RockPileRoom1</t>
-  </si>
-  <si>
-    <t>FindWoodenShieldRoom1</t>
-  </si>
-  <si>
-    <t>FindGoldRoom1</t>
-  </si>
-  <si>
-    <t>FindSmallKeyRoom1</t>
-  </si>
-  <si>
-    <t>FindArtofCombatRoom1</t>
-  </si>
-  <si>
-    <t>FindRepairVendorRoom1</t>
-  </si>
-  <si>
-    <t>EmptyCavePath3</t>
-  </si>
-  <si>
-    <t>FindGiantSnakeRoom1</t>
-  </si>
-  <si>
-    <t>FindSwordRoom1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>L1StartingRoom</t>
+  </si>
+  <si>
+    <t>L1MedicalOffice1</t>
+  </si>
+  <si>
+    <t>L1EncounterDyingDoctor</t>
+  </si>
+  <si>
+    <t>L1MedicalOffice2</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallE1</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallE2</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallES1</t>
+  </si>
+  <si>
+    <t>L1MedicalBay2</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallES2</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallES3</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallWS3</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallWS2</t>
+  </si>
+  <si>
+    <t>L1MedicalWingHallWS1</t>
+  </si>
+  <si>
+    <t>L1MainCorridorN1</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW1</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW2</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNE1</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW3</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW4</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW5</t>
+  </si>
+  <si>
+    <t>L1MainCorridorNW6</t>
+  </si>
+  <si>
+    <t>L1MessHall1</t>
+  </si>
+  <si>
+    <t>L1MessHall2</t>
+  </si>
+  <si>
+    <t>L1BarracksNW1</t>
+  </si>
+  <si>
+    <t>L1BarracksNW3</t>
+  </si>
+  <si>
+    <t>L1BarracksNW2</t>
   </si>
 </sst>
 </file>
@@ -125,11 +146,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,96 +433,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E12:K18"/>
+  <dimension ref="A3:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="H12" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E3" s="2"/>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="H13" t="s">
+      <c r="H6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
-        <v>4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
-      <c r="J15" t="s">
-        <v>3</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F16" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refined enemy logic including room descriptions, enemy attacks, and looting.  Added more map and items
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16640" yWindow="460" windowWidth="15980" windowHeight="18640" tabRatio="500"/>
+    <workbookView xWindow="22220" yWindow="460" windowWidth="23340" windowHeight="23840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map.txt" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>L1StartingRoom</t>
   </si>
@@ -105,16 +105,132 @@
   </si>
   <si>
     <t>L1BarracksNW2</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW7</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW8</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW9</t>
+  </si>
+  <si>
+    <t>L1BarracksNW4</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW10</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW11</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW12</t>
+  </si>
+  <si>
+    <t>L1BarracksNW5</t>
+  </si>
+  <si>
+    <t>L1MessHall3</t>
+  </si>
+  <si>
+    <t>L1MessHall4</t>
+  </si>
+  <si>
+    <t>L1MessHall5</t>
+  </si>
+  <si>
+    <t>L1MessHall6</t>
+  </si>
+  <si>
+    <t>L1MessHall7</t>
+  </si>
+  <si>
+    <t>L1BarracksNW6</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW13</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW14</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW15</t>
+  </si>
+  <si>
+    <t>L1WestStorageRoom1</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW16</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW17</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW18</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW21</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW20</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW19</t>
+  </si>
+  <si>
+    <t>L1BarracksNW7</t>
+  </si>
+  <si>
+    <t>L1BarracksNW8</t>
+  </si>
+  <si>
+    <t>L1BarracksNW9</t>
+  </si>
+  <si>
+    <t>L1BarracksNW10</t>
+  </si>
+  <si>
+    <t>L1BarracksNW11</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW22</t>
+  </si>
+  <si>
+    <t>L1WestCorridorNW23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +246,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -143,21 +259,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,16 +561,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
@@ -451,104 +580,491 @@
     <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E3" s="2"/>
-      <c r="G3" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H34" s="3"/>
+      <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more map segments, more narratives, minor bug fixes
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfarmer/Coding/com.despoina/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfarmer/Coding/com.europa/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22220" yWindow="460" windowWidth="23340" windowHeight="23840" tabRatio="500"/>
+    <workbookView xWindow="54340" yWindow="8920" windowWidth="31300" windowHeight="18540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map.txt" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>L1StartingRoom</t>
   </si>
@@ -197,7 +197,130 @@
     <t>L1WestCorridorNW22</t>
   </si>
   <si>
-    <t>L1WestCorridorNW23</t>
+    <t>L1CrawlSpaceNW1</t>
+  </si>
+  <si>
+    <t>L1CrawlSpaceNW2</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE2</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE3</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE4</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE5</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE6</t>
+  </si>
+  <si>
+    <t>L1EastCorridorNE7</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingHall1</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingHall2</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingHall3</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingHall4</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingCell1</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingCell2</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingCell3</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingCell4</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingCell5</t>
+  </si>
+  <si>
+    <t>L1ContainmentWingOffice1</t>
+  </si>
+  <si>
+    <t>L1WestCorridorMW1</t>
+  </si>
+  <si>
+    <t>L1WestCorridorMW2</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingHall1</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingHall2</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingHall3</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingHall4</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingHall5</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage1</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage2</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage3</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage1a</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage2a</t>
+  </si>
+  <si>
+    <t>L1ArmoryWingStorage3a</t>
+  </si>
+  <si>
+    <t>Crew Quarters</t>
+  </si>
+  <si>
+    <t>Space Walk Chamber</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>L2 Shipping/Receiving Dock</t>
+  </si>
+  <si>
+    <t>Bridge &amp; Command Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fitness &amp; Exercise </t>
+  </si>
+  <si>
+    <t>Greenhouse</t>
+  </si>
+  <si>
+    <t>External Space Walk</t>
+  </si>
+  <si>
+    <t>Cargo Hold</t>
+  </si>
+  <si>
+    <t>Engineering Bay / Reactor</t>
+  </si>
+  <si>
+    <t>Hypersleep Chambers</t>
   </si>
 </sst>
 </file>
@@ -236,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +372,48 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -259,7 +424,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -267,25 +432,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -561,26 +768,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -591,7 +800,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -602,31 +811,31 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -639,15 +848,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>12</v>
@@ -658,46 +866,46 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -724,64 +932,100 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="H9" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="1"/>
@@ -791,33 +1035,43 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="4" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="H13" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="1"/>
@@ -827,27 +1081,34 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="H14" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="M14" s="16"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -863,210 +1124,347 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="17"/>
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>56</v>
+      <c r="B17" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="M17" s="16"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="D18" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="M18" s="16"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="M19" s="16"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+      <c r="M20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="M21" s="16"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="M22" s="16"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>83</v>
+      </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>86</v>
+      </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H26" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="E32" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="13"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="H33" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="E36" s="15"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C37" s="15"/>
+      <c r="E37" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="16"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="16"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="H33:J36"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M12:M22"/>
+    <mergeCell ref="H26:J30"/>
+    <mergeCell ref="A28:C36"/>
+    <mergeCell ref="A38:C41"/>
+    <mergeCell ref="E37:G41"/>
+    <mergeCell ref="D18:F30"/>
+    <mergeCell ref="H15:J18"/>
+    <mergeCell ref="I21:J23"/>
+    <mergeCell ref="E32:F35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated install file, map and world, included setup changes to work on freezing package for windows
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54340" yWindow="8920" windowWidth="31300" windowHeight="18540" tabRatio="500"/>
+    <workbookView xWindow="2300" yWindow="560" windowWidth="31300" windowHeight="18540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map.txt" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>L1StartingRoom</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>Hypersleep Chambers</t>
+  </si>
+  <si>
+    <t>Communications Bay</t>
   </si>
 </sst>
 </file>
@@ -461,19 +464,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -768,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1041,7 +1044,7 @@
       <c r="I12" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="M12" s="16" t="s">
+      <c r="M12" s="17" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1065,7 +1068,7 @@
         <v>62</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="M13" s="16"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1085,7 +1088,7 @@
         <v>63</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1101,12 +1104,12 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="M15" s="16"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1124,14 +1127,14 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="17" t="s">
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="L16" s="17"/>
-      <c r="M16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
@@ -1143,10 +1146,10 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="M17" s="16"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
@@ -1155,17 +1158,17 @@
       <c r="B18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="13" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="M18" s="16"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -1173,13 +1176,13 @@
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="14"/>
+      <c r="H19" s="13"/>
       <c r="I19" s="1"/>
-      <c r="M19" s="16"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -1191,13 +1194,16 @@
       <c r="C20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="1"/>
-      <c r="M20" s="16"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -1205,16 +1211,14 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="13"/>
-      <c r="M21" s="16"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
@@ -1226,14 +1230,14 @@
       <c r="C22" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="M22" s="16"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
@@ -1241,13 +1245,11 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
@@ -1255,215 +1257,225 @@
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="1"/>
+      <c r="H24" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="1"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="14"/>
+      <c r="B27" s="13"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="14"/>
+      <c r="E31" s="13"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="1"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="13"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="14"/>
+      <c r="I33" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
       <c r="G34" s="1"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="E36" s="15"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="15"/>
-      <c r="E37" s="16" t="s">
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="E36" s="14"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C37" s="14"/>
+      <c r="E37" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="16"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="I38" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="H33:J36"/>
+  <mergeCells count="12">
     <mergeCell ref="K16:L16"/>
     <mergeCell ref="M12:M22"/>
-    <mergeCell ref="H26:J30"/>
+    <mergeCell ref="I38:K42"/>
     <mergeCell ref="A28:C36"/>
     <mergeCell ref="A38:C41"/>
     <mergeCell ref="E37:G41"/>
+    <mergeCell ref="I33:K36"/>
     <mergeCell ref="D18:F30"/>
     <mergeCell ref="H15:J18"/>
-    <mergeCell ref="I21:J23"/>
     <mergeCell ref="E32:F35"/>
+    <mergeCell ref="I20:J22"/>
+    <mergeCell ref="H24:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed readable issues, multi-interaction item usage issues, and gramma corrections in world
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -774,7 +774,7 @@
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,6 +877,9 @@
         <v>34</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
@@ -968,9 +971,6 @@
         <v>29</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>

<commit_message>
moved location of room back to correct location
</commit_message>
<xml_diff>
--- a/res/map.xlsx
+++ b/res/map.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfarmer/Coding/com.europa/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Corey Farmer\Downloads\europa\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -329,7 +329,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -503,6 +503,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -777,7 +780,7 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
@@ -792,7 +795,7 @@
     <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -803,7 +806,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -814,7 +817,7 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -826,7 +829,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>38</v>
       </c>
@@ -851,7 +854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
@@ -869,7 +872,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>22</v>
       </c>
@@ -877,9 +880,6 @@
         <v>34</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -911,7 +911,7 @@
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -938,7 +938,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -963,7 +963,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -971,6 +971,9 @@
         <v>29</v>
       </c>
       <c r="C10" s="1"/>
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -993,7 +996,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1070,7 +1073,7 @@
       <c r="I13" s="1"/>
       <c r="M13" s="17"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1090,7 +1093,7 @@
       <c r="I14" s="1"/>
       <c r="M14" s="17"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -1111,7 +1114,7 @@
       <c r="J15" s="18"/>
       <c r="M15" s="17"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1136,7 +1139,7 @@
       <c r="L16" s="16"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="9" t="s">
         <v>74</v>
@@ -1151,7 +1154,7 @@
       <c r="J17" s="18"/>
       <c r="M17" s="17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>76</v>
       </c>
@@ -1170,7 +1173,7 @@
       <c r="J18" s="18"/>
       <c r="M18" s="17"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>77</v>
       </c>
@@ -1184,7 +1187,7 @@
       <c r="I19" s="1"/>
       <c r="M19" s="17"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>78</v>
       </c>
@@ -1205,7 +1208,7 @@
       <c r="J20" s="18"/>
       <c r="M20" s="17"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>79</v>
       </c>
@@ -1220,7 +1223,7 @@
       <c r="J21" s="18"/>
       <c r="M21" s="17"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
@@ -1239,7 +1242,7 @@
       <c r="J22" s="18"/>
       <c r="M22" s="17"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>83</v>
       </c>
@@ -1251,7 +1254,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>86</v>
       </c>
@@ -1267,7 +1270,7 @@
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B25" s="13"/>
       <c r="C25" s="1"/>
       <c r="D25" s="18"/>
@@ -1278,7 +1281,7 @@
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1290,7 +1293,7 @@
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="13"/>
       <c r="C27" s="1"/>
@@ -1299,7 +1302,7 @@
       <c r="F27" s="18"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="s">
         <v>95</v>
       </c>
@@ -1310,7 +1313,7 @@
       <c r="F28" s="18"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -1319,7 +1322,7 @@
       <c r="F29" s="18"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -1328,7 +1331,7 @@
       <c r="F30" s="18"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -1338,7 +1341,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1350,7 +1353,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
@@ -1365,7 +1368,7 @@
       <c r="J33" s="17"/>
       <c r="K33" s="17"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
       <c r="C34" s="18"/>
@@ -1377,7 +1380,7 @@
       <c r="J34" s="17"/>
       <c r="K34" s="17"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -1387,7 +1390,7 @@
       <c r="J35" s="17"/>
       <c r="K35" s="17"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="18"/>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -1396,7 +1399,7 @@
       <c r="J36" s="17"/>
       <c r="K36" s="17"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C37" s="14"/>
       <c r="E37" s="17" t="s">
         <v>97</v>
@@ -1405,7 +1408,7 @@
       <c r="G37" s="17"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
         <v>96</v>
       </c>
@@ -1421,7 +1424,7 @@
       <c r="J38" s="18"/>
       <c r="K38" s="18"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -1433,7 +1436,7 @@
       <c r="J39" s="18"/>
       <c r="K39" s="18"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
@@ -1445,7 +1448,7 @@
       <c r="J40" s="18"/>
       <c r="K40" s="18"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="17"/>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
@@ -1457,7 +1460,7 @@
       <c r="J41" s="18"/>
       <c r="K41" s="18"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I42" s="18"/>
       <c r="J42" s="18"/>
       <c r="K42" s="18"/>

</xml_diff>